<commit_message>
Add more reference sequences
</commit_message>
<xml_diff>
--- a/8_Species_IDs.xlsx
+++ b/8_Species_IDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassiopea/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgold/Documents/GitHub/2025_Rockfish/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BF8C33E-DE94-6E49-801D-541F3121AEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD1DBA2-1A96-854A-8D32-46DD32EF2B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="1000" windowWidth="27640" windowHeight="16940" xr2:uid="{FBFB5118-A3CE-8A4B-8123-97005AB79773}"/>
+    <workbookView xWindow="2600" yWindow="1000" windowWidth="27640" windowHeight="16940" xr2:uid="{FBFB5118-A3CE-8A4B-8123-97005AB79773}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="153">
   <si>
     <t>species</t>
   </si>
@@ -455,36 +455,15 @@
     <t>4G5</t>
   </si>
   <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>E8</t>
   </si>
   <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
     <t>E10</t>
   </si>
   <si>
     <t>cut Sebastes_chrysomelas-EF446475.1_1_750?</t>
   </si>
   <si>
-    <t>3E11'</t>
-  </si>
-  <si>
     <t>Sebastes_hopkinsi-EF446448.1_1_750</t>
   </si>
   <si>
@@ -495,6 +474,27 @@
   </si>
   <si>
     <t>chrysomelas/carnatus identicle</t>
+  </si>
+  <si>
+    <t>1E11</t>
+  </si>
+  <si>
+    <t>3E11</t>
+  </si>
+  <si>
+    <t>3E9</t>
+  </si>
+  <si>
+    <t>2E2</t>
+  </si>
+  <si>
+    <t>2E7</t>
+  </si>
+  <si>
+    <t>2E4</t>
+  </si>
+  <si>
+    <t>1E3</t>
   </si>
 </sst>
 </file>
@@ -538,9 +538,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,15 +875,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A55C0D-854D-0746-9F9C-DE32C07D60A2}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:S120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -893,7 +896,7 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
@@ -903,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -913,7 +916,7 @@
       <c r="C2">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
@@ -926,10 +929,13 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="S2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -939,7 +945,7 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
@@ -951,8 +957,11 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -962,7 +971,7 @@
       <c r="C4">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
@@ -974,8 +983,11 @@
       <c r="G4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -985,7 +997,7 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
@@ -997,8 +1009,11 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1008,7 +1023,7 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E6" t="s">
@@ -1020,8 +1035,11 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1031,7 +1049,7 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
@@ -1043,8 +1061,11 @@
       <c r="G7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1054,7 +1075,7 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
@@ -1066,8 +1087,11 @@
       <c r="G8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1077,7 +1101,7 @@
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
@@ -1089,8 +1113,11 @@
       <c r="G9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1100,7 +1127,7 @@
       <c r="C10">
         <v>6</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E10" t="s">
@@ -1112,8 +1139,11 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1123,7 +1153,7 @@
       <c r="C11">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E11" t="s">
@@ -1135,8 +1165,11 @@
       <c r="G11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1146,8 +1179,8 @@
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>139</v>
+      <c r="D12" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -1158,8 +1191,11 @@
       <c r="G12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1169,7 +1205,7 @@
       <c r="C13">
         <v>7</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E13" t="s">
@@ -1181,8 +1217,11 @@
       <c r="G13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1192,7 +1231,7 @@
       <c r="C14">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E14" t="s">
@@ -1204,8 +1243,11 @@
       <c r="G14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1215,7 +1257,7 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E15" t="s">
@@ -1227,8 +1269,11 @@
       <c r="G15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="S15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1238,7 +1283,7 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E16" t="s">
@@ -1250,8 +1295,11 @@
       <c r="G16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1261,7 +1309,7 @@
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E17" t="s">
@@ -1273,8 +1321,11 @@
       <c r="G17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1284,7 +1335,7 @@
       <c r="C18">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E18" t="s">
@@ -1296,8 +1347,11 @@
       <c r="G18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1307,7 +1361,7 @@
       <c r="C19">
         <v>7</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E19" t="s">
@@ -1319,8 +1373,11 @@
       <c r="G19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1330,7 +1387,7 @@
       <c r="C20">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E20" t="s">
@@ -1342,8 +1399,11 @@
       <c r="G20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1353,7 +1413,7 @@
       <c r="C21">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E21" t="s">
@@ -1365,8 +1425,11 @@
       <c r="G21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1376,7 +1439,7 @@
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E22" t="s">
@@ -1388,8 +1451,11 @@
       <c r="G22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1399,7 +1465,7 @@
       <c r="C23">
         <v>11</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E23" t="s">
@@ -1411,8 +1477,11 @@
       <c r="G23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1422,7 +1491,7 @@
       <c r="C24">
         <v>11</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E24" t="s">
@@ -1434,8 +1503,11 @@
       <c r="G24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1445,7 +1517,7 @@
       <c r="C25">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E25" t="s">
@@ -1457,8 +1529,11 @@
       <c r="G25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1468,7 +1543,7 @@
       <c r="C26">
         <v>11</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E26" t="s">
@@ -1480,8 +1555,11 @@
       <c r="G26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1491,8 +1569,8 @@
       <c r="C27">
         <v>11</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>148</v>
+      <c r="D27" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
@@ -1503,8 +1581,11 @@
       <c r="G27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1514,7 +1595,7 @@
       <c r="C28">
         <v>3</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E28" t="s">
@@ -1526,8 +1607,11 @@
       <c r="G28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1537,8 +1621,8 @@
       <c r="C29">
         <v>9</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>140</v>
+      <c r="D29" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
@@ -1549,8 +1633,11 @@
       <c r="G29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1560,7 +1647,7 @@
       <c r="C30">
         <v>7</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E30" t="s">
@@ -1572,8 +1659,11 @@
       <c r="G30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1583,7 +1673,7 @@
       <c r="C31">
         <v>9</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E31" t="s">
@@ -1595,8 +1685,11 @@
       <c r="G31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1606,7 +1699,7 @@
       <c r="C32">
         <v>10</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E32" t="s">
@@ -1618,8 +1711,11 @@
       <c r="G32" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1629,7 +1725,7 @@
       <c r="C33">
         <v>11</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E33" t="s">
@@ -1641,8 +1737,11 @@
       <c r="G33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1652,7 +1751,7 @@
       <c r="C34">
         <v>12</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E34" t="s">
@@ -1664,8 +1763,11 @@
       <c r="G34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1675,7 +1777,7 @@
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E35" t="s">
@@ -1687,8 +1789,11 @@
       <c r="G35" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1698,7 +1803,7 @@
       <c r="C36">
         <v>3</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>52</v>
       </c>
       <c r="E36" t="s">
@@ -1710,8 +1815,11 @@
       <c r="G36" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1721,7 +1829,7 @@
       <c r="C37">
         <v>7</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E37" t="s">
@@ -1733,8 +1841,11 @@
       <c r="G37" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1744,7 +1855,7 @@
       <c r="C38">
         <v>12</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>54</v>
       </c>
       <c r="E38" t="s">
@@ -1756,8 +1867,11 @@
       <c r="G38" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1767,7 +1881,7 @@
       <c r="C39">
         <v>6</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E39" t="s">
@@ -1779,8 +1893,11 @@
       <c r="G39" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1790,8 +1907,8 @@
       <c r="C40">
         <v>2</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>141</v>
+      <c r="D40" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
@@ -1802,8 +1919,11 @@
       <c r="G40" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1813,8 +1933,8 @@
       <c r="C41">
         <v>8</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>142</v>
+      <c r="D41" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E41" t="s">
         <v>9</v>
@@ -1825,8 +1945,11 @@
       <c r="G41" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1836,7 +1959,7 @@
       <c r="C42">
         <v>12</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E42" t="s">
@@ -1848,8 +1971,11 @@
       <c r="G42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1859,8 +1985,8 @@
       <c r="C43">
         <v>7</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>143</v>
+      <c r="D43" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
@@ -1871,8 +1997,11 @@
       <c r="G43" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1882,8 +2011,8 @@
       <c r="C44">
         <v>4</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>144</v>
+      <c r="D44" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E44" t="s">
         <v>9</v>
@@ -1891,14 +2020,17 @@
       <c r="F44" t="s">
         <v>59</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1908,7 +2040,7 @@
       <c r="C45">
         <v>3</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E45" t="s">
@@ -1917,14 +2049,17 @@
       <c r="F45" t="s">
         <v>59</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I45" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1934,8 +2069,8 @@
       <c r="C46">
         <v>3</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>145</v>
+      <c r="D46" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="E46" t="s">
         <v>9</v>
@@ -1946,8 +2081,11 @@
       <c r="G46" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1957,7 +2095,7 @@
       <c r="C47">
         <v>7</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E47" t="s">
@@ -1969,8 +2107,11 @@
       <c r="G47" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1980,7 +2121,7 @@
       <c r="C48">
         <v>8</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>63</v>
       </c>
       <c r="E48" t="s">
@@ -1992,8 +2133,11 @@
       <c r="G48" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2003,7 +2147,7 @@
       <c r="C49">
         <v>10</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E49" t="s">
@@ -2015,8 +2159,11 @@
       <c r="G49" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -2026,7 +2173,7 @@
       <c r="C50">
         <v>12</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E50" t="s">
@@ -2038,8 +2185,11 @@
       <c r="G50" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2049,7 +2199,7 @@
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E51" t="s">
@@ -2061,8 +2211,11 @@
       <c r="G51" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -2072,7 +2225,7 @@
       <c r="C52">
         <v>3</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E52" t="s">
@@ -2081,11 +2234,14 @@
       <c r="F52" t="s">
         <v>59</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S52" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -2095,7 +2251,7 @@
       <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E53" t="s">
@@ -2107,8 +2263,11 @@
       <c r="G53" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -2118,7 +2277,7 @@
       <c r="C54">
         <v>4</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E54" t="s">
@@ -2130,8 +2289,11 @@
       <c r="G54" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -2141,7 +2303,7 @@
       <c r="C55">
         <v>6</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E55" t="s">
@@ -2153,8 +2315,11 @@
       <c r="G55" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -2164,7 +2329,7 @@
       <c r="C56">
         <v>8</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E56" t="s">
@@ -2176,8 +2341,11 @@
       <c r="G56" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -2187,7 +2355,7 @@
       <c r="C57">
         <v>9</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E57" t="s">
@@ -2199,8 +2367,11 @@
       <c r="G57" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -2210,7 +2381,7 @@
       <c r="C58">
         <v>12</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E58" t="s">
@@ -2222,8 +2393,11 @@
       <c r="G58" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -2233,7 +2407,7 @@
       <c r="C59">
         <v>3</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E59" t="s">
@@ -2245,8 +2419,11 @@
       <c r="G59" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -2256,7 +2433,7 @@
       <c r="C60">
         <v>10</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="2" t="s">
         <v>76</v>
       </c>
       <c r="E60" t="s">
@@ -2265,14 +2442,17 @@
       <c r="F60" t="s">
         <v>75</v>
       </c>
-      <c r="G60" s="3" t="s">
-        <v>151</v>
+      <c r="G60" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="I60" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -2282,7 +2462,7 @@
       <c r="C61">
         <v>11</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="2" t="s">
         <v>77</v>
       </c>
       <c r="E61" t="s">
@@ -2294,8 +2474,11 @@
       <c r="G61" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -2305,7 +2488,7 @@
       <c r="C62">
         <v>1</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E62" t="s">
@@ -2317,8 +2500,11 @@
       <c r="G62" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -2328,7 +2514,7 @@
       <c r="C63">
         <v>2</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E63" t="s">
@@ -2340,8 +2526,11 @@
       <c r="G63" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="S63" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -2351,7 +2540,7 @@
       <c r="C64">
         <v>4</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E64" t="s">
@@ -2363,8 +2552,11 @@
       <c r="G64" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2374,7 +2566,7 @@
       <c r="C65">
         <v>5</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E65" t="s">
@@ -2386,8 +2578,11 @@
       <c r="G65" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S65" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2397,7 +2592,7 @@
       <c r="C66">
         <v>8</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="2" t="s">
         <v>82</v>
       </c>
       <c r="E66" t="s">
@@ -2409,8 +2604,11 @@
       <c r="G66" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S66" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -2420,7 +2618,7 @@
       <c r="C67">
         <v>9</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E67" t="s">
@@ -2432,8 +2630,11 @@
       <c r="G67" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S67" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
@@ -2443,7 +2644,7 @@
       <c r="C68">
         <v>10</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="2" t="s">
         <v>84</v>
       </c>
       <c r="E68" t="s">
@@ -2455,8 +2656,11 @@
       <c r="G68" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>3</v>
       </c>
@@ -2466,7 +2670,7 @@
       <c r="C69">
         <v>3</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E69" t="s">
@@ -2478,8 +2682,11 @@
       <c r="G69" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S69" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>3</v>
       </c>
@@ -2489,7 +2696,7 @@
       <c r="C70">
         <v>4</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="2" t="s">
         <v>86</v>
       </c>
       <c r="E70" t="s">
@@ -2501,8 +2708,11 @@
       <c r="G70" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S70" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>3</v>
       </c>
@@ -2512,7 +2722,7 @@
       <c r="C71">
         <v>6</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E71" t="s">
@@ -2524,8 +2734,11 @@
       <c r="G71" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S71" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>4</v>
       </c>
@@ -2535,7 +2748,7 @@
       <c r="C72">
         <v>7</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E72" t="s">
@@ -2547,8 +2760,11 @@
       <c r="G72" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>4</v>
       </c>
@@ -2558,7 +2774,7 @@
       <c r="C73">
         <v>8</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="2" t="s">
         <v>89</v>
       </c>
       <c r="E73" t="s">
@@ -2570,8 +2786,11 @@
       <c r="G73" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>4</v>
       </c>
@@ -2581,7 +2800,7 @@
       <c r="C74">
         <v>9</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E74" t="s">
@@ -2593,8 +2812,11 @@
       <c r="G74" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4</v>
       </c>
@@ -2604,7 +2826,7 @@
       <c r="C75">
         <v>2</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E75" t="s">
@@ -2616,8 +2838,11 @@
       <c r="G75" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S75" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>4</v>
       </c>
@@ -2627,7 +2852,7 @@
       <c r="C76">
         <v>4</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E76" t="s">
@@ -2639,8 +2864,11 @@
       <c r="G76" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S76" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>4</v>
       </c>
@@ -2650,7 +2878,7 @@
       <c r="C77">
         <v>5</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E77" t="s">
@@ -2662,8 +2890,11 @@
       <c r="G77" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S77" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>4</v>
       </c>
@@ -2673,7 +2904,7 @@
       <c r="C78">
         <v>6</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="2" t="s">
         <v>94</v>
       </c>
       <c r="E78" t="s">
@@ -2685,8 +2916,11 @@
       <c r="G78" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S78" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>4</v>
       </c>
@@ -2696,7 +2930,7 @@
       <c r="C79">
         <v>10</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E79" t="s">
@@ -2708,8 +2942,11 @@
       <c r="G79" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>4</v>
       </c>
@@ -2719,7 +2956,7 @@
       <c r="C80">
         <v>11</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="2" t="s">
         <v>96</v>
       </c>
       <c r="E80" t="s">
@@ -2731,8 +2968,11 @@
       <c r="G80" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S80" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4</v>
       </c>
@@ -2742,7 +2982,7 @@
       <c r="C81">
         <v>1</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E81" t="s">
@@ -2754,8 +2994,11 @@
       <c r="G81" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>4</v>
       </c>
@@ -2765,7 +3008,7 @@
       <c r="C82">
         <v>12</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E82" t="s">
@@ -2777,8 +3020,11 @@
       <c r="G82" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S82" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>4</v>
       </c>
@@ -2788,7 +3034,7 @@
       <c r="C83">
         <v>2</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E83" t="s">
@@ -2800,8 +3046,11 @@
       <c r="G83" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S83" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>4</v>
       </c>
@@ -2811,7 +3060,7 @@
       <c r="C84">
         <v>3</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="2" t="s">
         <v>101</v>
       </c>
       <c r="E84" t="s">
@@ -2823,8 +3072,11 @@
       <c r="G84" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S84" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>4</v>
       </c>
@@ -2834,7 +3086,7 @@
       <c r="C85">
         <v>4</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="2" t="s">
         <v>102</v>
       </c>
       <c r="E85" t="s">
@@ -2846,8 +3098,11 @@
       <c r="G85" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S85" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>4</v>
       </c>
@@ -2857,7 +3112,7 @@
       <c r="C86">
         <v>5</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E86" t="s">
@@ -2869,8 +3124,11 @@
       <c r="G86" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S86" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>4</v>
       </c>
@@ -2880,7 +3138,7 @@
       <c r="C87">
         <v>6</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="2" t="s">
         <v>104</v>
       </c>
       <c r="E87" t="s">
@@ -2892,8 +3150,11 @@
       <c r="G87" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S87" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>4</v>
       </c>
@@ -2903,7 +3164,7 @@
       <c r="C88">
         <v>7</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E88" t="s">
@@ -2915,8 +3176,11 @@
       <c r="G88" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S88" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>4</v>
       </c>
@@ -2926,7 +3190,7 @@
       <c r="C89">
         <v>8</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E89" t="s">
@@ -2938,8 +3202,11 @@
       <c r="G89" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S89" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>4</v>
       </c>
@@ -2949,7 +3216,7 @@
       <c r="C90">
         <v>9</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="2" t="s">
         <v>108</v>
       </c>
       <c r="E90" t="s">
@@ -2961,8 +3228,11 @@
       <c r="G90" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S90" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2972,7 +3242,7 @@
       <c r="C91">
         <v>5</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E91" t="s">
@@ -2984,8 +3254,11 @@
       <c r="G91" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S91" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>4</v>
       </c>
@@ -2995,7 +3268,7 @@
       <c r="C92">
         <v>6</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E92" t="s">
@@ -3007,8 +3280,11 @@
       <c r="G92" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S92" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>4</v>
       </c>
@@ -3018,7 +3294,7 @@
       <c r="C93">
         <v>7</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E93" t="s">
@@ -3030,8 +3306,11 @@
       <c r="G93" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S93" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>4</v>
       </c>
@@ -3041,7 +3320,7 @@
       <c r="C94">
         <v>8</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E94" t="s">
@@ -3053,8 +3332,11 @@
       <c r="G94" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S94" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>4</v>
       </c>
@@ -3064,7 +3346,7 @@
       <c r="C95">
         <v>4</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E95" t="s">
@@ -3076,8 +3358,11 @@
       <c r="G95" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S95" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>4</v>
       </c>
@@ -3087,7 +3372,7 @@
       <c r="C96">
         <v>2</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="2" t="s">
         <v>114</v>
       </c>
       <c r="E96" t="s">
@@ -3099,8 +3384,11 @@
       <c r="G96" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S96" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>4</v>
       </c>
@@ -3110,7 +3398,7 @@
       <c r="C97">
         <v>6</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E97" t="s">
@@ -3122,8 +3410,11 @@
       <c r="G97" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S97" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>4</v>
       </c>
@@ -3133,7 +3424,7 @@
       <c r="C98">
         <v>12</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E98" t="s">
@@ -3145,8 +3436,11 @@
       <c r="G98" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S98" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>4</v>
       </c>
@@ -3156,7 +3450,7 @@
       <c r="C99">
         <v>1</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E99" t="s">
@@ -3168,8 +3462,11 @@
       <c r="G99" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>4</v>
       </c>
@@ -3179,7 +3476,7 @@
       <c r="C100">
         <v>2</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="2" t="s">
         <v>119</v>
       </c>
       <c r="E100" t="s">
@@ -3191,8 +3488,11 @@
       <c r="G100" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S100" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>4</v>
       </c>
@@ -3202,7 +3502,7 @@
       <c r="C101">
         <v>3</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E101" t="s">
@@ -3214,8 +3514,11 @@
       <c r="G101" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S101" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>4</v>
       </c>
@@ -3225,7 +3528,7 @@
       <c r="C102">
         <v>4</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E102" t="s">
@@ -3237,8 +3540,11 @@
       <c r="G102" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S102" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>4</v>
       </c>
@@ -3248,7 +3554,7 @@
       <c r="C103">
         <v>5</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E103" t="s">
@@ -3260,8 +3566,11 @@
       <c r="G103" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S103" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>4</v>
       </c>
@@ -3271,7 +3580,7 @@
       <c r="C104">
         <v>6</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="2" t="s">
         <v>123</v>
       </c>
       <c r="E104" t="s">
@@ -3283,8 +3592,11 @@
       <c r="G104" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S104" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>4</v>
       </c>
@@ -3294,7 +3606,7 @@
       <c r="C105">
         <v>7</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="2" t="s">
         <v>124</v>
       </c>
       <c r="E105" t="s">
@@ -3306,8 +3618,11 @@
       <c r="G105" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S105" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>4</v>
       </c>
@@ -3317,7 +3632,7 @@
       <c r="C106">
         <v>9</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="2" t="s">
         <v>125</v>
       </c>
       <c r="E106" t="s">
@@ -3329,8 +3644,11 @@
       <c r="G106" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S106" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>4</v>
       </c>
@@ -3340,7 +3658,7 @@
       <c r="C107">
         <v>11</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E107" t="s">
@@ -3352,8 +3670,11 @@
       <c r="G107" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S107" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>4</v>
       </c>
@@ -3363,7 +3684,7 @@
       <c r="C108">
         <v>10</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="2" t="s">
         <v>127</v>
       </c>
       <c r="E108" t="s">
@@ -3375,8 +3696,11 @@
       <c r="G108" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S108" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>4</v>
       </c>
@@ -3386,7 +3710,7 @@
       <c r="C109">
         <v>12</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="2" t="s">
         <v>128</v>
       </c>
       <c r="E109" t="s">
@@ -3398,8 +3722,11 @@
       <c r="G109" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>4</v>
       </c>
@@ -3409,8 +3736,8 @@
       <c r="C110">
         <v>10</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>146</v>
+      <c r="D110" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="E110" t="s">
         <v>9</v>
@@ -3421,8 +3748,11 @@
       <c r="G110" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>4</v>
       </c>
@@ -3432,7 +3762,7 @@
       <c r="C111">
         <v>3</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="2" t="s">
         <v>129</v>
       </c>
       <c r="E111" t="s">
@@ -3444,8 +3774,11 @@
       <c r="G111" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S111" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>4</v>
       </c>
@@ -3455,7 +3788,7 @@
       <c r="C112">
         <v>4</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="2" t="s">
         <v>130</v>
       </c>
       <c r="E112" t="s">
@@ -3467,8 +3800,11 @@
       <c r="G112" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S112" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>4</v>
       </c>
@@ -3478,7 +3814,7 @@
       <c r="C113">
         <v>5</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="2" t="s">
         <v>131</v>
       </c>
       <c r="E113" t="s">
@@ -3490,8 +3826,11 @@
       <c r="G113" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S113" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>4</v>
       </c>
@@ -3501,7 +3840,7 @@
       <c r="C114">
         <v>1</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E114" t="s">
@@ -3513,8 +3852,11 @@
       <c r="G114" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S114" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>4</v>
       </c>
@@ -3524,7 +3866,7 @@
       <c r="C115">
         <v>12</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E115" t="s">
@@ -3536,8 +3878,11 @@
       <c r="G115" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>4</v>
       </c>
@@ -3547,7 +3892,7 @@
       <c r="C116">
         <v>9</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E116" t="s">
@@ -3559,8 +3904,11 @@
       <c r="G116" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>4</v>
       </c>
@@ -3570,7 +3918,7 @@
       <c r="C117">
         <v>10</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E117" t="s">
@@ -3582,8 +3930,11 @@
       <c r="G117" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>4</v>
       </c>
@@ -3593,7 +3944,7 @@
       <c r="C118">
         <v>3</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="2" t="s">
         <v>136</v>
       </c>
       <c r="E118" t="s">
@@ -3605,8 +3956,11 @@
       <c r="G118" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S118" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>4</v>
       </c>
@@ -3616,7 +3970,7 @@
       <c r="C119">
         <v>2</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="2" t="s">
         <v>137</v>
       </c>
       <c r="E119" t="s">
@@ -3628,8 +3982,11 @@
       <c r="G119" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="S119" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>4</v>
       </c>
@@ -3639,7 +3996,7 @@
       <c r="C120">
         <v>5</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="2" t="s">
         <v>138</v>
       </c>
       <c r="E120" t="s">
@@ -3649,6 +4006,9 @@
         <v>28</v>
       </c>
       <c r="G120" t="s">
+        <v>28</v>
+      </c>
+      <c r="S120" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>